<commit_message>
fixed streamflow rating curve
</commit_message>
<xml_diff>
--- a/data-dict.xlsx
+++ b/data-dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizacohn/Desktop/cascaded-hydro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB0BD7B-1748-D94B-B537-A6A17BB5C99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536963A1-6F0A-DF45-882F-9776455D5526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="760" windowWidth="28740" windowHeight="17060" xr2:uid="{91E4E570-4FDA-D248-8E42-05C4D408F481}"/>
+    <workbookView xWindow="180" yWindow="760" windowWidth="28740" windowHeight="16920" xr2:uid="{91E4E570-4FDA-D248-8E42-05C4D408F481}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD51759A-88E3-AC40-9138-3704E9D6A5FC}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="124" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
convex hull approx begin;'
</commit_message>
<xml_diff>
--- a/data-dict.xlsx
+++ b/data-dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizacohn/Desktop/cascaded-hydro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA38CDD8-E3D0-A94B-B831-E9FE142537A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25880A4D-AD16-994A-861B-1A33D73DFE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="760" windowWidth="28740" windowHeight="16920" xr2:uid="{91E4E570-4FDA-D248-8E42-05C4D408F481}"/>
+    <workbookView xWindow="180" yWindow="760" windowWidth="28740" windowHeight="16920" activeTab="1" xr2:uid="{91E4E570-4FDA-D248-8E42-05C4D408F481}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -902,7 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD51759A-88E3-AC40-9138-3704E9D6A5FC}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="124" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="124" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1350,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0B08DC-B182-A544-B60A-AB068FE2E834}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1732,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61B70D3-5C38-3445-B4CB-083D2E3B0506}">
   <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>

</xml_diff>